<commit_message>
added ratio of drug arrest/part time normal
</commit_message>
<xml_diff>
--- a/modifiedWorkbook.xlsx
+++ b/modifiedWorkbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misha\Documents\GitHub\fork\483Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C405C9CA-41CF-42F5-8CE8-694632DC700B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5483D7C-AAF1-4434-8824-989D2A065E29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="577" yWindow="480" windowWidth="15556" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2033" yWindow="1425" windowWidth="15555" windowHeight="12105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toronto Wellbeing Data" sheetId="1" r:id="rId1"/>
@@ -1556,7 +1556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
@@ -7074,8 +7074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18756738-B0CE-48E1-B7C0-42B597FECA32}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>